<commit_message>
Subí PSP Clase Usuario y BD_Usuario
</commit_message>
<xml_diff>
--- a/Documentación/Psp's/Salma/BD Usuario/Defectos removidos.xlsx
+++ b/Documentación/Psp's/Salma/BD Usuario/Defectos removidos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yosse\Documents\TSP\PSP\Psp BD Usuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yosse\Downloads\Clase BD_Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E4178D-63E6-4D09-B439-38DC0BA01319}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAC8B320-E1CE-4321-9EE8-CD13470DBDDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
-    <sheet name="excel(3)" sheetId="1" r:id="rId1"/>
+    <sheet name="excel(4)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="excel_3" localSheetId="0">'excel(3)'!$A$1:$E$28</definedName>
+    <definedName name="excel_4" localSheetId="0">'excel(4)'!$A$1:$E$25</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -24,14 +24,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\Yosse\Downloads\excel(3).iqy" name="excel(3)" type="4" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" odcFile="C:\Users\Yosse\Downloads\Clase BD_Usuario\excel(4).iqy" name="excel(4)" type="4" refreshedVersion="6" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://localhost:2469/reports/form2html.class?uri=%2FProyecto%2FPSP2%2E1Clase%2BBD%2BUsuario%2F%2Fcms%2Fpsp2%2E1%2Fsummary%3Fframe%3Dcontent%26section%3D111&amp;EXPORT=excel" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>/Proyecto/PSP2.1Clase BD Usuario</t>
   </si>
@@ -39,12 +39,6 @@
     <t>PSP2.1 Project Plan Summary</t>
   </si>
   <si>
-    <t>El PROBE Wizard usa la EstimaciÃ³n de TamaÃ±o de Proxy como la base para generar estimados finales para el tiempo y tamaÃ±o. Sin embargo, despuÃ©s de que corriste el Wizard por Ãºltima vez, modificaste los estimados en la plantilla de EstimaciÃ³n de Tiempo, causando que el TamaÃ±o de Proxy Estimado cambiara. Su estimado PROBE actual estÃ¡ basado en un valor antiguo de TamaÃ±o de Proxy Estimado. Para resolver este problema, debe revisar los valores en la Plantilla de EstimaciÃ³n de TamaÃ±o, y correr el Wizard de nuevo</t>
-  </si>
-  <si>
-    <t>Debe ingresar datos actuales de tamaÃ±o para este proyecto.</t>
-  </si>
-  <si>
     <t>Defects Removed</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>PlaneaciÃ³n</t>
   </si>
   <si>
-    <t>#DIV/0!</t>
-  </si>
-  <si>
     <t>DiseÃ±o</t>
   </si>
   <si>
@@ -93,7 +84,7 @@
     <t>Adapted from "PSP Materials," copyright © 2006 Carnegie Mellon University. Used by permission.</t>
   </si>
   <si>
-    <t>Reporte generado a las 11:36 AM el 22/11/2018</t>
+    <t>Reporte generado a las 09:03 PM el 4/12/2018</t>
   </si>
 </sst>
 </file>
@@ -624,7 +615,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -634,9 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -652,6 +640,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -718,7 +712,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel(3)" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel(4)" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1018,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1047,207 +1041,194 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.23100000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B12" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>7.6899999999999996E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>10</v>
+      <c r="B13" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.46200000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>10</v>
+      <c r="B14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.154</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>0.4</v>
       </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>10</v>
+      <c r="C15" s="7">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>7.6899999999999996E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
-        <v>2.4</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="B16" s="8">
+        <v>5.19</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="C17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="C18" s="8">
-        <v>2</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="B19" s="9">
-        <v>5.19</v>
-      </c>
-      <c r="C19" s="8">
-        <v>3</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>